<commit_message>
Complete All Game Logic Fix several bugs in event card UI and add cost display for event cards. Fix bug when equipment attribute is importing from CSV. Import all the category and attribute
</commit_message>
<xml_diff>
--- a/Assets/DataBase/Data/DataSet.xlsx
+++ b/Assets/DataBase/Data/DataSet.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="592">
   <si>
     <t>工作类型</t>
   </si>
@@ -1284,6 +1284,9 @@
     <t>0.15*0.05</t>
   </si>
   <si>
+    <t>0*2</t>
+  </si>
+  <si>
     <t>15*12</t>
   </si>
   <si>
@@ -1311,15 +1314,24 @@
     <t>55*5</t>
   </si>
   <si>
+    <t>1*4</t>
+  </si>
+  <si>
     <t>18*14</t>
   </si>
   <si>
     <t>6*4</t>
   </si>
   <si>
+    <t>1*5</t>
+  </si>
+  <si>
     <t>8*3</t>
   </si>
   <si>
+    <t>1*3</t>
+  </si>
+  <si>
     <t>10*0</t>
   </si>
   <si>
@@ -1329,6 +1341,9 @@
     <t>Spell</t>
   </si>
   <si>
+    <t>1*6</t>
+  </si>
+  <si>
     <t>5*0</t>
   </si>
   <si>
@@ -1341,6 +1356,9 @@
     <t>70*10</t>
   </si>
   <si>
+    <t>1*2*5</t>
+  </si>
+  <si>
     <t>45*5</t>
   </si>
   <si>
@@ -1350,6 +1368,9 @@
     <t>60*5</t>
   </si>
   <si>
+    <t>2*5</t>
+  </si>
+  <si>
     <t>极慢-VerySlow</t>
   </si>
   <si>
@@ -1377,16 +1398,25 @@
     <t>13*0</t>
   </si>
   <si>
+    <t>3*7</t>
+  </si>
+  <si>
     <t>16*14</t>
   </si>
   <si>
     <t>15*15</t>
   </si>
   <si>
+    <t>8*5</t>
+  </si>
+  <si>
     <t>16*20</t>
   </si>
   <si>
     <t>9*5</t>
+  </si>
+  <si>
+    <t>6*2</t>
   </si>
   <si>
     <t>R-尸体-1-4,R-奴隶-1-3,R-灵魂-1-3</t>
@@ -3351,13 +3381,13 @@
 <file path=xl/woinfos.xml><?xml version="1.0" encoding="utf-8"?>
 <woInfos xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookInfo cellCmpFml="0">
-    <open main="172" threadCnt="1"/>
+    <open main="235" threadCnt="1"/>
     <sheetInfos>
       <sheetInfo cellCmpFml="0" sheetStid="2">
-        <open threadCnt="1"/>
+        <open main="1" threadCnt="1"/>
       </sheetInfo>
       <sheetInfo cellCmpFml="0" sheetStid="6">
-        <open main="58" threadCnt="1"/>
+        <open main="63" threadCnt="1"/>
       </sheetInfo>
       <sheetInfo cellCmpFml="0" sheetStid="7">
         <open main="1" threadCnt="1"/>
@@ -5946,7 +5976,9 @@
       <c r="Q8" s="55">
         <v>20</v>
       </c>
-      <c r="R8" s="57"/>
+      <c r="R8" s="57">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" s="51" customFormat="1" spans="1:18">
       <c r="A9" s="55" t="s">
@@ -6002,7 +6034,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="10" s="51" customFormat="1" spans="1:17">
+    <row r="10" s="51" customFormat="1" spans="1:18">
       <c r="A10" s="55" t="s">
         <v>17</v>
       </c>
@@ -6052,6 +6084,9 @@
       <c r="Q10" s="55">
         <v>20</v>
       </c>
+      <c r="R10" s="57" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="11" s="51" customFormat="1" spans="1:18">
       <c r="A11" s="55" t="s">
@@ -6070,19 +6105,19 @@
         <v>378</v>
       </c>
       <c r="F11" s="51" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G11" s="55" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H11" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I11" s="58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J11" s="57" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K11" s="55" t="s">
         <v>387</v>
@@ -6097,7 +6132,7 @@
         <v>361</v>
       </c>
       <c r="O11" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P11" s="55" t="s">
         <v>384</v>
@@ -6106,10 +6141,10 @@
         <v>35</v>
       </c>
       <c r="R11" s="57" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="12" s="51" customFormat="1" spans="1:17">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="12" s="51" customFormat="1" spans="1:18">
       <c r="A12" s="55" t="s">
         <v>25</v>
       </c>
@@ -6123,22 +6158,22 @@
         <v>377</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="G12" s="55" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H12" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I12" s="58" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J12" s="57" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K12" s="55" t="s">
         <v>372</v>
@@ -6153,7 +6188,7 @@
         <v>361</v>
       </c>
       <c r="O12" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P12" s="55" t="s">
         <v>384</v>
@@ -6161,8 +6196,11 @@
       <c r="Q12" s="55">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" s="51" customFormat="1" spans="1:17">
+      <c r="R12" s="57" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" s="51" customFormat="1" spans="1:18">
       <c r="A13" s="55" t="s">
         <v>29</v>
       </c>
@@ -6176,22 +6214,22 @@
         <v>377</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="G13" s="55" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="H13" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I13" s="58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J13" s="57" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K13" s="55" t="s">
         <v>372</v>
@@ -6206,7 +6244,7 @@
         <v>361</v>
       </c>
       <c r="O13" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P13" s="55" t="s">
         <v>384</v>
@@ -6214,8 +6252,11 @@
       <c r="Q13" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" s="51" customFormat="1" spans="1:17">
+      <c r="R13" s="57" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="14" s="51" customFormat="1" spans="1:18">
       <c r="A14" s="55" t="s">
         <v>31</v>
       </c>
@@ -6229,22 +6270,22 @@
         <v>377</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="G14" s="55" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H14" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I14" s="58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J14" s="57" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K14" s="55" t="s">
         <v>387</v>
@@ -6259,7 +6300,7 @@
         <v>361</v>
       </c>
       <c r="O14" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P14" s="55" t="s">
         <v>367</v>
@@ -6267,8 +6308,11 @@
       <c r="Q14" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" s="51" customFormat="1" spans="1:17">
+      <c r="R14" s="57" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" s="51" customFormat="1" spans="1:18">
       <c r="A15" s="55" t="s">
         <v>33</v>
       </c>
@@ -6282,22 +6326,22 @@
         <v>377</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F15" s="51" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="G15" s="55" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H15" s="51" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="I15" s="58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J15" s="57" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K15" s="55" t="s">
         <v>372</v>
@@ -6309,19 +6353,22 @@
         <v>387</v>
       </c>
       <c r="N15" s="51" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="O15" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P15" s="55" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="Q15" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" s="51" customFormat="1" spans="1:17">
+      <c r="R15" s="57" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="16" s="51" customFormat="1" spans="1:18">
       <c r="A16" s="55" t="s">
         <v>35</v>
       </c>
@@ -6335,22 +6382,22 @@
         <v>377</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="F16" s="51" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="G16" s="55" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="H16" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I16" s="58" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="J16" s="57" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="K16" s="55" t="s">
         <v>372</v>
@@ -6365,7 +6412,7 @@
         <v>361</v>
       </c>
       <c r="O16" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P16" s="55" t="s">
         <v>384</v>
@@ -6373,8 +6420,11 @@
       <c r="Q16" s="55">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" s="51" customFormat="1" spans="1:17">
+      <c r="R16" s="57" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="17" s="51" customFormat="1" spans="1:18">
       <c r="A17" s="55" t="s">
         <v>37</v>
       </c>
@@ -6400,16 +6450,16 @@
         <v>370</v>
       </c>
       <c r="I17" s="58" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="J17" s="57" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="K17" s="55" t="s">
         <v>383</v>
       </c>
       <c r="L17" s="51" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="M17" s="55" t="s">
         <v>387</v>
@@ -6418,7 +6468,7 @@
         <v>361</v>
       </c>
       <c r="O17" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P17" s="55" t="s">
         <v>384</v>
@@ -6426,8 +6476,11 @@
       <c r="Q17" s="55">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" s="51" customFormat="1" spans="1:17">
+      <c r="R17" s="57" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" s="51" customFormat="1" spans="1:18">
       <c r="A18" s="55" t="s">
         <v>39</v>
       </c>
@@ -6441,22 +6494,22 @@
         <v>377</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="F18" s="57" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G18" s="58" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H18" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I18" s="58" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="J18" s="57" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="K18" s="55" t="s">
         <v>387</v>
@@ -6471,7 +6524,7 @@
         <v>361</v>
       </c>
       <c r="O18" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P18" s="55" t="s">
         <v>384</v>
@@ -6479,8 +6532,11 @@
       <c r="Q18" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" s="51" customFormat="1" spans="1:17">
+      <c r="R18" s="57" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="19" s="51" customFormat="1" spans="1:18">
       <c r="A19" s="55" t="s">
         <v>41</v>
       </c>
@@ -6488,7 +6544,7 @@
         <v>369</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D19" s="51" t="s">
         <v>355</v>
@@ -6497,22 +6553,22 @@
         <v>370</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="G19" s="58" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="H19" s="51" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="I19" s="58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="J19" s="57" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="K19" s="55" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="L19" s="51" t="s">
         <v>370</v>
@@ -6524,7 +6580,7 @@
         <v>361</v>
       </c>
       <c r="O19" s="55" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="P19" s="55" t="s">
         <v>384</v>
@@ -6532,8 +6588,11 @@
       <c r="Q19" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" s="51" customFormat="1" spans="1:17">
+      <c r="R19" s="57" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" s="51" customFormat="1" spans="1:18">
       <c r="A20" s="55" t="s">
         <v>43</v>
       </c>
@@ -6541,7 +6600,7 @@
         <v>369</v>
       </c>
       <c r="C20" s="55" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D20" s="51" t="s">
         <v>355</v>
@@ -6550,22 +6609,22 @@
         <v>370</v>
       </c>
       <c r="F20" s="57" t="s">
+        <v>415</v>
+      </c>
+      <c r="G20" s="58" t="s">
+        <v>428</v>
+      </c>
+      <c r="H20" s="51" t="s">
         <v>410</v>
       </c>
-      <c r="G20" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="H20" s="51" t="s">
-        <v>406</v>
-      </c>
       <c r="I20" s="58" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="J20" s="57" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="K20" s="55" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="L20" s="51" t="s">
         <v>370</v>
@@ -6577,7 +6636,7 @@
         <v>361</v>
       </c>
       <c r="O20" s="55" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="P20" s="55" t="s">
         <v>384</v>
@@ -6585,8 +6644,11 @@
       <c r="Q20" s="55">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" s="19" customFormat="1" spans="1:17">
+      <c r="R20" s="57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" s="19" customFormat="1" spans="1:18">
       <c r="A21" s="55" t="s">
         <v>45</v>
       </c>
@@ -6606,19 +6668,19 @@
         <v>379</v>
       </c>
       <c r="G21" s="55" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="H21" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I21" s="58" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="J21" s="57" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="K21" s="55" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="L21" s="51" t="s">
         <v>388</v>
@@ -6627,10 +6689,10 @@
         <v>372</v>
       </c>
       <c r="N21" s="51" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="O21" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P21" s="55" t="s">
         <v>384</v>
@@ -6638,8 +6700,11 @@
       <c r="Q21" s="55">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" s="19" customFormat="1" spans="1:17">
+      <c r="R21" s="27" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="22" s="19" customFormat="1" spans="1:18">
       <c r="A22" s="55" t="s">
         <v>47</v>
       </c>
@@ -6653,22 +6718,22 @@
         <v>377</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="G22" s="55" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H22" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I22" s="58" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J22" s="57" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K22" s="55" t="s">
         <v>374</v>
@@ -6683,7 +6748,7 @@
         <v>361</v>
       </c>
       <c r="O22" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P22" s="55" t="s">
         <v>384</v>
@@ -6691,8 +6756,11 @@
       <c r="Q22" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" s="19" customFormat="1" spans="1:17">
+      <c r="R22" s="27" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="23" s="19" customFormat="1" spans="1:18">
       <c r="A23" s="55" t="s">
         <v>49</v>
       </c>
@@ -6706,22 +6774,22 @@
         <v>377</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="G23" s="55" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H23" s="51" t="s">
         <v>370</v>
       </c>
       <c r="I23" s="58" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="K23" s="55" t="s">
         <v>387</v>
@@ -6736,7 +6804,7 @@
         <v>361</v>
       </c>
       <c r="O23" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P23" s="55" t="s">
         <v>384</v>
@@ -6744,8 +6812,11 @@
       <c r="Q23" s="55">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" s="19" customFormat="1" spans="1:17">
+      <c r="R23" s="27" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="24" s="19" customFormat="1" spans="1:18">
       <c r="A24" s="55" t="s">
         <v>51</v>
       </c>
@@ -6759,22 +6830,22 @@
         <v>377</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="G24" s="55" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="I24" s="58" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="J24" s="57" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="K24" s="55" t="s">
         <v>372</v>
@@ -6789,13 +6860,16 @@
         <v>361</v>
       </c>
       <c r="O24" s="55" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="P24" s="55" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="Q24" s="55">
         <v>60</v>
+      </c>
+      <c r="R24" s="27" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="25" s="19" customFormat="1" spans="1:17">
@@ -6803,13 +6877,13 @@
         <v>53</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>370</v>
@@ -6842,7 +6916,7 @@
         <v>361</v>
       </c>
       <c r="O25" s="26" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="P25" s="15" t="s">
         <v>384</v>
@@ -6856,22 +6930,22 @@
         <v>55</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>370</v>
       </c>
       <c r="F26" s="27" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>370</v>
@@ -6895,7 +6969,7 @@
         <v>361</v>
       </c>
       <c r="O26" s="26" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="P26" s="15" t="s">
         <v>384</v>
@@ -6906,16 +6980,16 @@
     </row>
     <row r="27" s="19" customFormat="1" spans="1:17">
       <c r="A27" s="26" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>370</v>
@@ -6930,10 +7004,10 @@
         <v>370</v>
       </c>
       <c r="I27" s="26" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="K27" s="26" t="s">
         <v>387</v>
@@ -6948,7 +7022,7 @@
         <v>378</v>
       </c>
       <c r="O27" s="26" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="P27" s="26" t="s">
         <v>384</v>
@@ -6959,16 +7033,16 @@
     </row>
     <row r="28" s="19" customFormat="1" spans="1:17">
       <c r="A28" s="26" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>370</v>
@@ -6977,7 +7051,7 @@
         <v>371</v>
       </c>
       <c r="G28" s="26" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="H28" s="27" t="s">
         <v>370</v>
@@ -7001,7 +7075,7 @@
         <v>361</v>
       </c>
       <c r="O28" s="26" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="P28" s="26" t="s">
         <v>384</v>
@@ -7012,22 +7086,22 @@
     </row>
     <row r="29" s="19" customFormat="1" spans="1:17">
       <c r="A29" s="26" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>370</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="G29" s="26" t="s">
         <v>372</v>
@@ -7036,16 +7110,16 @@
         <v>370</v>
       </c>
       <c r="I29" s="26" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="J29" s="27" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="K29" s="26" t="s">
         <v>387</v>
       </c>
       <c r="L29" s="27" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="M29" s="26" t="s">
         <v>372</v>
@@ -7054,10 +7128,10 @@
         <v>361</v>
       </c>
       <c r="O29" s="26" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="P29" s="26" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="Q29" s="15">
         <v>200</v>
@@ -7065,16 +7139,16 @@
     </row>
     <row r="30" s="19" customFormat="1" spans="1:17">
       <c r="A30" s="26" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>370</v>
@@ -7089,10 +7163,10 @@
         <v>361</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="J30" s="27" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="K30" s="26" t="s">
         <v>374</v>
@@ -7107,7 +7181,7 @@
         <v>361</v>
       </c>
       <c r="O30" s="26" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="P30" s="26" t="s">
         <v>367</v>
@@ -7121,19 +7195,19 @@
         <v>57</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>370</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>380</v>
@@ -7142,10 +7216,10 @@
         <v>370</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>387</v>
@@ -7160,7 +7234,7 @@
         <v>361</v>
       </c>
       <c r="O31" s="15" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="P31" s="15" t="s">
         <v>384</v>
@@ -7174,34 +7248,34 @@
         <v>59</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>370</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>370</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="L32" s="19" t="s">
         <v>370</v>
@@ -7213,7 +7287,7 @@
         <v>361</v>
       </c>
       <c r="O32" s="26" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="P32" s="15" t="s">
         <v>384</v>
@@ -7227,34 +7301,34 @@
         <v>61</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>370</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="H33" s="19" t="s">
         <v>370</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="L33" s="19" t="s">
         <v>370</v>
@@ -7263,10 +7337,10 @@
         <v>374</v>
       </c>
       <c r="N33" s="19" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="O33" s="26" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="P33" s="15" t="s">
         <v>384</v>
@@ -7280,22 +7354,22 @@
         <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D34" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E34" s="54" t="s">
         <v>370</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="G34" s="54" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="H34" s="56" t="s">
         <v>370</v>
@@ -7319,7 +7393,7 @@
         <v>361</v>
       </c>
       <c r="O34" s="54" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>384</v>
@@ -7363,36 +7437,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="32" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" s="19" customFormat="1" spans="1:5">
       <c r="A2" s="23" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>465</v>
+        <v>475</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>466</v>
+        <v>476</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>467</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" s="19" customFormat="1" spans="1:5">
@@ -7400,13 +7474,13 @@
         <v>334</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="E3" s="43" t="s">
         <v>335</v>
@@ -7417,10 +7491,10 @@
         <v>334</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>335</v>
@@ -7432,7 +7506,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C5" s="29">
         <v>999</v>
@@ -7446,7 +7520,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C6" s="29">
         <v>1</v>
@@ -7460,7 +7534,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C7" s="29">
         <v>1</v>
@@ -7477,7 +7551,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C8" s="29">
         <v>1</v>
@@ -7491,7 +7565,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C9" s="29">
         <v>1</v>
@@ -7505,7 +7579,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C10" s="29">
         <v>1</v>
@@ -7519,7 +7593,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C11" s="29">
         <v>999</v>
@@ -7533,7 +7607,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C12" s="29">
         <v>3</v>
@@ -7547,7 +7621,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C13" s="29">
         <v>3</v>
@@ -7561,7 +7635,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C14" s="29">
         <v>1</v>
@@ -7575,7 +7649,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C15" s="29">
         <v>1</v>
@@ -7589,7 +7663,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C16" s="29">
         <v>1</v>
@@ -7603,7 +7677,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C17" s="29">
         <v>1</v>
@@ -7620,7 +7694,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C18" s="29">
         <v>1</v>
@@ -7637,7 +7711,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C19" s="29">
         <v>3</v>
@@ -7654,7 +7728,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C20" s="29">
         <v>1</v>
@@ -7665,10 +7739,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="42" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C21" s="29">
         <v>1</v>
@@ -7682,7 +7756,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C22" s="29">
         <v>1</v>
@@ -7696,7 +7770,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C23" s="29">
         <v>999</v>
@@ -7710,7 +7784,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C24" s="29">
         <v>999</v>
@@ -7724,7 +7798,7 @@
         <v>58</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C25" s="29">
         <v>1</v>
@@ -7738,7 +7812,7 @@
         <v>60</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C26" s="29">
         <v>1</v>
@@ -7752,7 +7826,7 @@
         <v>62</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C27" s="29">
         <v>1</v>
@@ -7766,7 +7840,7 @@
         <v>64</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C28" s="29">
         <v>999</v>
@@ -7780,7 +7854,7 @@
         <v>66</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C29" s="29">
         <v>1</v>
@@ -7794,7 +7868,7 @@
         <v>67</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C30" s="29">
         <v>999</v>
@@ -7808,7 +7882,7 @@
         <v>68</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C31" s="29">
         <v>999</v>
@@ -7822,7 +7896,7 @@
         <v>69</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C32" s="29">
         <v>999</v>
@@ -7836,7 +7910,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C33" s="29">
         <v>1</v>
@@ -7850,7 +7924,7 @@
         <v>71</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C34" s="29">
         <v>999</v>
@@ -7864,7 +7938,7 @@
         <v>72</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C35" s="29">
         <v>1</v>
@@ -7878,7 +7952,7 @@
         <v>73</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C36" s="29">
         <v>1</v>
@@ -7892,7 +7966,7 @@
         <v>74</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C37" s="29">
         <v>1</v>
@@ -7906,7 +7980,7 @@
         <v>75</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C38" s="29">
         <v>1</v>
@@ -7920,7 +7994,7 @@
         <v>76</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C39" s="29">
         <v>999</v>
@@ -7934,7 +8008,7 @@
         <v>77</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="C40" s="29">
         <v>999</v>
@@ -7948,7 +8022,7 @@
         <v>78</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="C41" s="29">
         <v>2</v>
@@ -7965,7 +8039,7 @@
         <v>79</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="C42" s="29">
         <v>999</v>
@@ -7979,7 +8053,7 @@
         <v>80</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C43" s="29">
         <v>999</v>
@@ -7993,7 +8067,7 @@
         <v>81</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C44" s="29">
         <v>999</v>
@@ -8007,7 +8081,7 @@
         <v>82</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C45" s="29">
         <v>999</v>
@@ -8021,7 +8095,7 @@
         <v>83</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C46" s="29">
         <v>999</v>
@@ -8035,7 +8109,7 @@
         <v>84</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C47" s="29">
         <v>999</v>
@@ -8049,7 +8123,7 @@
         <v>85</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C48" s="29">
         <v>999</v>
@@ -8063,7 +8137,7 @@
         <v>86</v>
       </c>
       <c r="B49" s="47" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="C49" s="29">
         <v>999</v>
@@ -8132,7 +8206,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="20" t="s">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>303</v>
@@ -8164,7 +8238,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="15" t="s">
-        <v>479</v>
+        <v>489</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>321</v>
@@ -8196,7 +8270,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="15" t="s">
-        <v>480</v>
+        <v>490</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>336</v>
@@ -8213,13 +8287,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="15" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>482</v>
+        <v>492</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>482</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -8235,7 +8309,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="24" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
       <c r="B6" s="25">
         <v>1</v>
@@ -8678,7 +8752,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>484</v>
+        <v>494</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>96</v>
@@ -8699,13 +8773,13 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="1" t="s">
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8714,10 +8788,10 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="1" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>104</v>
@@ -8728,10 +8802,10 @@
         <v>-1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>491</v>
+        <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -8739,7 +8813,7 @@
         <v>-1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>492</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -8755,7 +8829,7 @@
         <v>-1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>493</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -8775,10 +8849,10 @@
         <v>5</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>495</v>
+        <v>505</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -8795,15 +8869,15 @@
         <v>15</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="15" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="D11" s="3">
         <v>700</v>
@@ -8812,10 +8886,10 @@
         <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -8832,15 +8906,15 @@
         <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>499</v>
+        <v>509</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="15" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="D13" s="3">
         <v>700</v>
@@ -8849,10 +8923,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -8869,30 +8943,30 @@
         <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>496</v>
+        <v>506</v>
       </c>
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="15" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>502</v>
+        <v>512</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="15" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>15</v>
@@ -8900,16 +8974,16 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="15" t="s">
-        <v>497</v>
+        <v>507</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>501</v>
+        <v>511</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -8933,10 +9007,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
     </row>
     <row r="21" ht="40.5" spans="1:3">
@@ -8947,7 +9021,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>505</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -8963,7 +9037,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -8971,7 +9045,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
     </row>
     <row r="25" ht="40.5" spans="1:3">
@@ -8979,10 +9053,10 @@
         <v>11</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>508</v>
+        <v>518</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>509</v>
+        <v>519</v>
       </c>
     </row>
     <row r="26" ht="27" spans="1:3">
@@ -8990,10 +9064,10 @@
         <v>12</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
     </row>
     <row r="27" ht="27" spans="1:3">
@@ -9001,10 +9075,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>513</v>
+        <v>523</v>
       </c>
     </row>
     <row r="28" ht="81" spans="1:3">
@@ -9012,10 +9086,10 @@
         <v>14</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>515</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" ht="54" spans="1:3">
@@ -9023,10 +9097,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>516</v>
+        <v>526</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>517</v>
+        <v>527</v>
       </c>
     </row>
     <row r="30" ht="67.5" spans="1:3">
@@ -9034,10 +9108,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>518</v>
+        <v>528</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
     </row>
     <row r="31" ht="27" spans="1:3">
@@ -9045,10 +9119,10 @@
         <v>17</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>521</v>
+        <v>531</v>
       </c>
     </row>
     <row r="32" ht="67.5" spans="1:3">
@@ -9056,10 +9130,10 @@
         <v>18</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>522</v>
+        <v>532</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -9067,10 +9141,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>524</v>
+        <v>534</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>525</v>
+        <v>535</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -9078,10 +9152,10 @@
         <v>20</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>526</v>
+        <v>536</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>527</v>
+        <v>537</v>
       </c>
     </row>
     <row r="35" ht="54" spans="1:3">
@@ -9089,10 +9163,10 @@
         <v>21</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
     </row>
     <row r="36" ht="27" spans="1:3">
@@ -9100,10 +9174,10 @@
         <v>22</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>531</v>
+        <v>541</v>
       </c>
     </row>
     <row r="37" ht="27" spans="1:3">
@@ -9111,10 +9185,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>532</v>
+        <v>542</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>533</v>
+        <v>543</v>
       </c>
     </row>
     <row r="38" ht="40.5" spans="1:3">
@@ -9122,10 +9196,10 @@
         <v>24</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>535</v>
+        <v>545</v>
       </c>
     </row>
     <row r="39" ht="27" spans="1:3">
@@ -9133,10 +9207,10 @@
         <v>25</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>537</v>
+        <v>547</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -9144,10 +9218,10 @@
         <v>26</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>538</v>
+        <v>548</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>539</v>
+        <v>549</v>
       </c>
     </row>
     <row r="41" ht="27" spans="1:3">
@@ -9158,7 +9232,7 @@
         <v>70</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>540</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -9166,10 +9240,10 @@
         <v>28</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>541</v>
+        <v>551</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>542</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" ht="27" spans="1:3">
@@ -9177,10 +9251,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>543</v>
+        <v>553</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>544</v>
+        <v>554</v>
       </c>
     </row>
     <row r="44" ht="27" spans="1:3">
@@ -9188,10 +9262,10 @@
         <v>30</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>546</v>
+        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -9199,10 +9273,10 @@
         <v>31</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>547</v>
+        <v>557</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>548</v>
+        <v>558</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -9210,10 +9284,10 @@
         <v>32</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>549</v>
+        <v>559</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
     </row>
     <row r="47" ht="40.5" spans="1:3">
@@ -9221,10 +9295,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
     </row>
     <row r="48" ht="27" spans="1:3">
@@ -9232,10 +9306,10 @@
         <v>34</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
     </row>
     <row r="49" ht="27" spans="1:3">
@@ -9246,7 +9320,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>555</v>
+        <v>565</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -9254,10 +9328,10 @@
         <v>36</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>556</v>
+        <v>566</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>557</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" ht="27" spans="1:3">
@@ -9265,10 +9339,10 @@
         <v>37</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>559</v>
+        <v>569</v>
       </c>
     </row>
     <row r="52" ht="27" spans="1:3">
@@ -9276,10 +9350,10 @@
         <v>38</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>561</v>
+        <v>571</v>
       </c>
     </row>
     <row r="53" ht="27" spans="1:3">
@@ -9287,10 +9361,10 @@
         <v>39</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
     </row>
     <row r="54" ht="40.5" spans="1:3">
@@ -9298,10 +9372,10 @@
         <v>40</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>564</v>
+        <v>574</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -9312,7 +9386,7 @@
         <v>44</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
     </row>
     <row r="56" ht="54" spans="1:3">
@@ -9320,10 +9394,10 @@
         <v>42</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>567</v>
+        <v>577</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>568</v>
+        <v>578</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -9331,7 +9405,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>569</v>
+        <v>579</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -9339,10 +9413,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -9350,7 +9424,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -9358,7 +9432,7 @@
         <v>46</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>573</v>
+        <v>583</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -9366,7 +9440,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>574</v>
+        <v>584</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -9374,7 +9448,7 @@
         <v>48</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -9382,7 +9456,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -9390,7 +9464,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>577</v>
+        <v>587</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -9406,7 +9480,7 @@
         <v>52</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>578</v>
+        <v>588</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -9422,10 +9496,10 @@
         <v>54</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -9433,7 +9507,7 @@
         <v>55</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve the illustrations in the design doc Add shader and material for flowy noise effect Fix Start Battle button not updating interactable state FINALL COMMIT
</commit_message>
<xml_diff>
--- a/Assets/DataBase/Data/DataSet.xlsx
+++ b/Assets/DataBase/Data/DataSet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="27945" windowHeight="12375" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="图鉴" sheetId="2" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="593">
   <si>
     <t>工作类型</t>
   </si>
@@ -471,7 +471,7 @@
     <t>R-王座厅探索点-1,C-Any-1</t>
   </si>
   <si>
-    <t>R-废铁-1-30,R-木料-1-25,R-野生蘑菇丛-1-20,R-土壤-1-1</t>
+    <t>R-废铁-1-30,R-木料-1-25,R-野生蘑菇丛-1-20,R-土壤-1-2</t>
   </si>
   <si>
     <t>浅层探索</t>
@@ -651,7 +651,7 @@
     <t>R-深层隧道网-1,C-Any-1</t>
   </si>
   <si>
-    <t>R-土壤-1-3,R-金币-1-8,R-银矿石-1-15,R-金矿石-1-10,R-贵重矿脉-1-15</t>
+    <t>R-土壤-1-1,R-金币-1-8,R-银矿石-1-15,R-金矿石-1-10,R-贵重矿脉-1-15</t>
   </si>
   <si>
     <t>切割石砖</t>
@@ -753,7 +753,7 @@
     <t>R-废铁-2,C-Any-1</t>
   </si>
   <si>
-    <t>R-废铁工具-1-10</t>
+    <t>R-废铁武器-1-10</t>
   </si>
   <si>
     <t>R-废铁-1,R-铁矿石-1,C-Any-1</t>
@@ -1372,7 +1372,7 @@
     <t>24*0</t>
   </si>
   <si>
-    <t>R-超大石料-2-10</t>
+    <t>R-石料-4-10</t>
   </si>
   <si>
     <t>14*3</t>
@@ -1408,16 +1408,16 @@
     <t>6*2</t>
   </si>
   <si>
-    <t>R-尸体-1-4,R-奴隶-1-3,R-灵魂-1-3</t>
-  </si>
-  <si>
-    <t>R-尸体-1-5,R-奴隶-1-2,R-灵魂-1-3</t>
+    <t>R-尸体-1-6,R-奴隶-1-3</t>
+  </si>
+  <si>
+    <t>R-尸体-1-4,R-奴隶-1-3</t>
   </si>
   <si>
     <t>60*0</t>
   </si>
   <si>
-    <t>R-尸体-1-4,R-金币-1-4,R-灵魂-1-3</t>
+    <t>R-尸体-1-4,R-金币-1-4</t>
   </si>
   <si>
     <t>R-烈酒-1-4,R-金币-1-6</t>
@@ -1465,7 +1465,7 @@
     <t>50*15</t>
   </si>
   <si>
-    <t>R-尸体-1-5,R-肉食-2-5</t>
+    <t>R-尸体-1-5,R-灵魂-1-5</t>
   </si>
   <si>
     <t>150*0</t>
@@ -1480,7 +1480,22 @@
     <t>2*1</t>
   </si>
   <si>
-    <t>R-灵魂-1-8,R-金币-1-2</t>
+    <t>R-灵魂-1-10</t>
+  </si>
+  <si>
+    <t>巨鼠（二级）</t>
+  </si>
+  <si>
+    <t>0*1</t>
+  </si>
+  <si>
+    <t>8*0</t>
+  </si>
+  <si>
+    <t>9*1</t>
+  </si>
+  <si>
+    <t>R-灵魂-1-7,R-金币-1-3</t>
   </si>
   <si>
     <t>ResourceType</t>
@@ -2864,7 +2879,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3145,9 +3160,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3440,13 +3452,13 @@
 <file path=xl/woinfos.xml><?xml version="1.0" encoding="utf-8"?>
 <woInfos xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookInfo cellCmpFml="0">
-    <open main="170" threadCnt="1"/>
+    <open main="307" threadCnt="1"/>
     <sheetInfos>
       <sheetInfo cellCmpFml="0" sheetStid="2">
-        <open threadCnt="1"/>
+        <open main="1" threadCnt="1"/>
       </sheetInfo>
       <sheetInfo cellCmpFml="0" sheetStid="6">
-        <open main="57" threadCnt="1"/>
+        <open main="99" threadCnt="1"/>
       </sheetInfo>
       <sheetInfo cellCmpFml="0" sheetStid="7">
         <open main="1" threadCnt="1"/>
@@ -3732,7 +3744,7 @@
   <sheetPr/>
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -3755,7 +3767,7 @@
       <c r="D1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="96" t="s">
+      <c r="E1" s="95" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3772,7 +3784,7 @@
       <c r="D2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="97" t="s">
+      <c r="E2" s="96" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3961,7 +3973,7 @@
       <c r="B22" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="94" t="s">
+      <c r="C22" s="90" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3991,13 +4003,13 @@
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="89"/>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="94" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="89"/>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="94" t="s">
         <v>65</v>
       </c>
     </row>
@@ -4013,7 +4025,7 @@
       <c r="B29" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="94" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4021,7 +4033,7 @@
       <c r="B30" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="94" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4069,27 +4081,27 @@
       </c>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="97" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="97" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="97" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="98" t="s">
+      <c r="B42" s="97" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="97" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4149,7 +4161,7 @@
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="98" t="s">
+      <c r="B55" s="97" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4189,8 +4201,8 @@
   <sheetPr/>
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G74"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="G44" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -4338,7 +4350,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" ht="14.25" spans="1:7">
+    <row r="10" spans="1:7">
       <c r="A10" s="62">
         <v>1</v>
       </c>
@@ -4359,7 +4371,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" ht="15" spans="1:7">
+    <row r="11" spans="1:7">
       <c r="A11" s="66">
         <v>2</v>
       </c>
@@ -4380,7 +4392,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" ht="15" spans="1:7">
       <c r="A12" s="66">
         <v>3</v>
       </c>
@@ -4548,7 +4560,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" ht="15" spans="1:7">
       <c r="A20" s="73">
         <v>11</v>
       </c>
@@ -4569,7 +4581,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" ht="15" spans="1:7">
       <c r="A21" s="73">
         <v>12</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" ht="15" spans="1:7">
       <c r="A22" s="73">
         <v>13</v>
       </c>
@@ -4737,7 +4749,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" ht="15" spans="1:7">
       <c r="A29" s="73">
         <v>20</v>
       </c>
@@ -4758,7 +4770,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" ht="15" spans="1:7">
+    <row r="30" spans="1:7">
       <c r="A30" s="73">
         <v>21</v>
       </c>
@@ -4779,7 +4791,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="31" ht="15" spans="1:7">
+    <row r="31" spans="1:7">
       <c r="A31" s="73">
         <v>21</v>
       </c>
@@ -4800,7 +4812,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="32" ht="15" spans="1:7">
+    <row r="32" spans="1:7">
       <c r="A32" s="73">
         <v>22</v>
       </c>
@@ -4842,7 +4854,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" ht="15" spans="1:7">
       <c r="A34" s="73">
         <v>24</v>
       </c>
@@ -4863,7 +4875,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" ht="15" spans="1:7">
       <c r="A35" s="73">
         <v>25</v>
       </c>
@@ -4884,7 +4896,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" ht="15" spans="1:7">
       <c r="A36" s="73">
         <v>26</v>
       </c>
@@ -5069,7 +5081,7 @@
       <c r="F44" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="G44" s="68" t="s">
+      <c r="G44" s="76" t="s">
         <v>223</v>
       </c>
     </row>
@@ -5723,10 +5735,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="F2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:N5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
@@ -6711,7 +6723,7 @@
       <c r="N19" s="50" t="s">
         <v>363</v>
       </c>
-      <c r="O19" s="54" t="s">
+      <c r="O19" s="57" t="s">
         <v>429</v>
       </c>
       <c r="P19" s="54" t="s">
@@ -6767,7 +6779,7 @@
       <c r="N20" s="50" t="s">
         <v>363</v>
       </c>
-      <c r="O20" s="54" t="s">
+      <c r="O20" s="57" t="s">
         <v>429</v>
       </c>
       <c r="P20" s="54" t="s">
@@ -7534,14 +7546,67 @@
         <v>200</v>
       </c>
     </row>
+    <row r="35" spans="1:17">
+      <c r="A35" s="53" t="s">
+        <v>466</v>
+      </c>
+      <c r="B35" t="s">
+        <v>425</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D35" t="s">
+        <v>425</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>467</v>
+      </c>
+      <c r="F35" s="55" t="s">
+        <v>468</v>
+      </c>
+      <c r="G35" s="53" t="s">
+        <v>402</v>
+      </c>
+      <c r="H35" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="I35" s="53" t="s">
+        <v>394</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>372</v>
+      </c>
+      <c r="K35" s="53" t="s">
+        <v>469</v>
+      </c>
+      <c r="L35" s="55" t="s">
+        <v>467</v>
+      </c>
+      <c r="M35" s="53" t="s">
+        <v>364</v>
+      </c>
+      <c r="N35" s="55" t="s">
+        <v>362</v>
+      </c>
+      <c r="O35" s="53" t="s">
+        <v>470</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q35" s="15">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P25:P1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34:B35 C34:C35 D34:D35 B6:D7 B25:D33 B36:D1048576">
+      <formula1>"狂热-Frenzy,快速-Fast,普通-Normal,缓慢-Slow,极慢-VerySlow"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P25:P33 P34:P35 P36:P1048576">
       <formula1>"Physical,Spell,TrueDamage"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:D7 B25:D1048576">
-      <formula1>"狂热-Frenzy,快速-Fast,普通-Normal,缓慢-Slow,极慢-VerySlow"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7569,36 +7634,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="32" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2" s="19" customFormat="1" spans="1:5">
       <c r="A2" s="23" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" s="19" customFormat="1" spans="1:5">
@@ -7606,13 +7671,13 @@
         <v>336</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="E3" s="43" t="s">
         <v>337</v>
@@ -7623,10 +7688,10 @@
         <v>336</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>337</v>
@@ -7638,7 +7703,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C5" s="29">
         <v>999</v>
@@ -7652,7 +7717,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C6" s="29">
         <v>999</v>
@@ -7666,7 +7731,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C7" s="29">
         <v>999</v>
@@ -7680,7 +7745,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C8" s="29">
         <v>999</v>
@@ -7694,7 +7759,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C9" s="29">
         <v>999</v>
@@ -7708,10 +7773,10 @@
         <v>28</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C10" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="31">
         <v>0</v>
@@ -7722,7 +7787,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C11" s="29">
         <v>999</v>
@@ -7736,7 +7801,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C12" s="29">
         <v>999</v>
@@ -7750,7 +7815,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C13" s="29">
         <v>1</v>
@@ -7767,7 +7832,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C14" s="29">
         <v>1</v>
@@ -7781,7 +7846,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C15" s="29">
         <v>1</v>
@@ -7798,7 +7863,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C16" s="29">
         <v>1</v>
@@ -7812,7 +7877,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C17" s="29">
         <v>1</v>
@@ -7829,7 +7894,7 @@
         <v>42</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C18" s="29">
         <v>1</v>
@@ -7846,7 +7911,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C19" s="29">
         <v>1</v>
@@ -7863,7 +7928,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="C20" s="29">
         <v>1</v>
@@ -7880,7 +7945,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C21" s="29">
         <v>1</v>
@@ -7894,7 +7959,7 @@
         <v>50</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C22" s="29">
         <v>1</v>
@@ -7908,7 +7973,7 @@
         <v>52</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C23" s="29">
         <v>1</v>
@@ -7922,7 +7987,7 @@
         <v>54</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C24" s="29">
         <v>1</v>
@@ -7936,7 +8001,7 @@
         <v>56</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C25" s="29">
         <v>1</v>
@@ -7950,7 +8015,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C26" s="29">
         <v>1</v>
@@ -7964,7 +8029,7 @@
         <v>60</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C27" s="29">
         <v>1</v>
@@ -7978,7 +8043,7 @@
         <v>62</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C28" s="29">
         <v>1</v>
@@ -7998,7 +8063,7 @@
         <v>66</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C31" s="29">
         <v>1</v>
@@ -8012,7 +8077,7 @@
         <v>68</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C32" s="29">
         <v>3</v>
@@ -8026,7 +8091,7 @@
         <v>70</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C33" s="29">
         <v>3</v>
@@ -8040,7 +8105,7 @@
         <v>72</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C34" s="29">
         <v>1</v>
@@ -8054,7 +8119,7 @@
         <v>74</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C35" s="29">
         <v>1</v>
@@ -8068,7 +8133,7 @@
         <v>75</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C36" s="29">
         <v>1</v>
@@ -8082,7 +8147,7 @@
         <v>76</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C37" s="29">
         <v>1</v>
@@ -8096,7 +8161,7 @@
         <v>77</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C38" s="29">
         <v>1</v>
@@ -8110,7 +8175,7 @@
         <v>78</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C39" s="29">
         <v>1</v>
@@ -8124,7 +8189,7 @@
         <v>79</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C40" s="29">
         <v>999</v>
@@ -8138,7 +8203,7 @@
         <v>80</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C41" s="29">
         <v>999</v>
@@ -8152,7 +8217,7 @@
         <v>81</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C42" s="29">
         <v>999</v>
@@ -8166,7 +8231,7 @@
         <v>82</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C43" s="29">
         <v>999</v>
@@ -8180,7 +8245,7 @@
         <v>83</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C44" s="29">
         <v>999</v>
@@ -8194,7 +8259,7 @@
         <v>84</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C45" s="29">
         <v>999</v>
@@ -8208,7 +8273,7 @@
         <v>85</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C46" s="29">
         <v>999</v>
@@ -8222,7 +8287,7 @@
         <v>86</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C47" s="29">
         <v>1</v>
@@ -8236,7 +8301,7 @@
         <v>87</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C48" s="29">
         <v>999</v>
@@ -8250,7 +8315,7 @@
         <v>88</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C49" s="29">
         <v>999</v>
@@ -8264,7 +8329,7 @@
         <v>89</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C50" s="29">
         <v>999</v>
@@ -8278,7 +8343,7 @@
         <v>90</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C51" s="29">
         <v>999</v>
@@ -8292,7 +8357,7 @@
         <v>91</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C52" s="29">
         <v>999</v>
@@ -8306,7 +8371,7 @@
         <v>92</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C53" s="29">
         <v>999</v>
@@ -8320,7 +8385,7 @@
         <v>93</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C54" s="29">
         <v>999</v>
@@ -8334,7 +8399,7 @@
         <v>94</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C55" s="29">
         <v>999</v>
@@ -8348,7 +8413,7 @@
         <v>95</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C56" s="29">
         <v>999</v>
@@ -8362,7 +8427,7 @@
         <v>96</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="C57" s="29">
         <v>999</v>
@@ -8376,7 +8441,7 @@
         <v>97</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C58" s="29">
         <v>1</v>
@@ -8390,7 +8455,7 @@
         <v>98</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C59" s="29">
         <v>1</v>
@@ -8404,7 +8469,7 @@
         <v>99</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C60" s="29">
         <v>1</v>
@@ -8452,7 +8517,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="20" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>305</v>
@@ -8484,7 +8549,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="15" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>323</v>
@@ -8516,7 +8581,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="15" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>338</v>
@@ -8533,13 +8598,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="15" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -8555,7 +8620,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="24" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B6" s="25">
         <v>1</v>
@@ -8998,7 +9063,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>109</v>
@@ -9019,13 +9084,13 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="1" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -9034,10 +9099,10 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="1" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>117</v>
@@ -9048,10 +9113,10 @@
         <v>-1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -9059,7 +9124,7 @@
         <v>-1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -9075,7 +9140,7 @@
         <v>-1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -9095,10 +9160,10 @@
         <v>5</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -9115,15 +9180,15 @@
         <v>15</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="15" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D11" s="3">
         <v>700</v>
@@ -9132,10 +9197,10 @@
         <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -9152,15 +9217,15 @@
         <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="15" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D13" s="3">
         <v>700</v>
@@ -9169,10 +9234,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -9189,30 +9254,30 @@
         <v>15</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="15" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="15" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>15</v>
@@ -9220,16 +9285,16 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="15" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -9253,10 +9318,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="21" ht="40.5" spans="1:3">
@@ -9264,10 +9329,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -9291,7 +9356,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25" ht="40.5" spans="1:3">
@@ -9299,10 +9364,10 @@
         <v>11</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="26" ht="27" spans="1:3">
@@ -9310,10 +9375,10 @@
         <v>12</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
     </row>
     <row r="27" ht="27" spans="1:3">
@@ -9321,10 +9386,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
     </row>
     <row r="28" ht="81" spans="1:3">
@@ -9332,10 +9397,10 @@
         <v>14</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
     </row>
     <row r="29" ht="54" spans="1:3">
@@ -9343,10 +9408,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
     </row>
     <row r="30" ht="67.5" spans="1:3">
@@ -9354,10 +9419,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" ht="27" spans="1:3">
@@ -9365,10 +9430,10 @@
         <v>17</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
     </row>
     <row r="32" ht="67.5" spans="1:3">
@@ -9379,7 +9444,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -9387,10 +9452,10 @@
         <v>19</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -9398,10 +9463,10 @@
         <v>20</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
     </row>
     <row r="35" ht="54" spans="1:3">
@@ -9409,10 +9474,10 @@
         <v>21</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="36" ht="27" spans="1:3">
@@ -9420,10 +9485,10 @@
         <v>22</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
     </row>
     <row r="37" ht="27" spans="1:3">
@@ -9431,10 +9496,10 @@
         <v>23</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
     <row r="38" ht="40.5" spans="1:3">
@@ -9442,10 +9507,10 @@
         <v>24</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
     </row>
     <row r="39" ht="27" spans="1:3">
@@ -9453,10 +9518,10 @@
         <v>25</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -9464,10 +9529,10 @@
         <v>26</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
     </row>
     <row r="41" ht="27" spans="1:3">
@@ -9478,7 +9543,7 @@
         <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -9489,7 +9554,7 @@
         <v>99</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
     </row>
     <row r="43" ht="27" spans="1:3">
@@ -9497,10 +9562,10 @@
         <v>29</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
     </row>
     <row r="44" ht="27" spans="1:3">
@@ -9508,10 +9573,10 @@
         <v>30</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -9519,10 +9584,10 @@
         <v>31</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -9530,10 +9595,10 @@
         <v>32</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="47" ht="40.5" spans="1:3">
@@ -9541,10 +9606,10 @@
         <v>33</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
     </row>
     <row r="48" ht="27" spans="1:3">
@@ -9552,10 +9617,10 @@
         <v>34</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
     </row>
     <row r="49" ht="27" spans="1:3">
@@ -9566,7 +9631,7 @@
         <v>34</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -9574,10 +9639,10 @@
         <v>36</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" ht="27" spans="1:3">
@@ -9585,10 +9650,10 @@
         <v>37</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
     </row>
     <row r="52" ht="27" spans="1:3">
@@ -9596,10 +9661,10 @@
         <v>38</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="53" ht="27" spans="1:3">
@@ -9607,10 +9672,10 @@
         <v>39</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="54" ht="40.5" spans="1:3">
@@ -9618,10 +9683,10 @@
         <v>40</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -9632,7 +9697,7 @@
         <v>40</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="56" ht="54" spans="1:3">
@@ -9640,10 +9705,10 @@
         <v>42</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -9651,7 +9716,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -9659,10 +9724,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -9670,7 +9735,7 @@
         <v>45</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -9678,7 +9743,7 @@
         <v>46</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -9686,7 +9751,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -9694,7 +9759,7 @@
         <v>48</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -9702,7 +9767,7 @@
         <v>49</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -9710,7 +9775,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -9718,7 +9783,7 @@
         <v>51</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -9726,7 +9791,7 @@
         <v>52</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -9742,10 +9807,10 @@
         <v>54</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -9753,7 +9818,7 @@
         <v>55</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
   </sheetData>

</xml_diff>